<commit_message>
V model for secondary writing on xlsx working
</commit_message>
<xml_diff>
--- a/Code/Data/Secondary_value.xlsx
+++ b/Code/Data/Secondary_value.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanwei/Documents/MATLAB/Space EVDT 2.0/Space-EVDT/Code/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{644CAB91-5666-0B4F-98B9-A42B5C86EDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26B79EF-8829-E14B-A956-CCE23F4BDAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CB8B1E65-7EE9-2C4E-A127-257EE0137411}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,13 +35,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -58,7 +54,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -66,12 +62,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -90,7 +88,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -241,7 +239,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -265,9 +263,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -291,7 +289,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -326,7 +324,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -344,7 +342,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -369,7 +367,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -405,37 +403,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B5D223-5ABE-D343-A7F1-A29E0BE91818}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B5D223-5ABE-D343-A7F1-A29E0BE91818}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="true" zoomScale="125" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="true"/>
+    <col min="5" max="5" width="2.7109375" customWidth="true"/>
+    <col min="6" max="9" width="2.6640625" customWidth="true"/>
+    <col min="10" max="10" width="6.6640625" customWidth="true"/>
+    <col min="11" max="14" width="2.6640625" customWidth="true"/>
+    <col min="2" max="2" width="2.7109375" customWidth="true"/>
+    <col min="3" max="3" width="2.7109375" customWidth="true"/>
+    <col min="4" max="4" width="2.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="0">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0">
         <v>2</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="0">
         <v>3</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="0">
         <v>4</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="0">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>35932</v>
+      </c>
+      <c r="B2" s="0">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>3048</v>
+      </c>
+      <c r="B3" s="0">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V model working with V based Decision model
</commit_message>
<xml_diff>
--- a/Code/Data/Secondary_value.xlsx
+++ b/Code/Data/Secondary_value.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanwei/Documents/MATLAB/Space EVDT 2.0/Space-EVDT/Code/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26B79EF-8829-E14B-A956-CCE23F4BDAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222051E1-5E70-A648-A7FB-608B148B6815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" fullCalcOnLoad="true"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,8 +36,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -54,7 +54,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -62,14 +62,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -88,7 +86,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -239,7 +237,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -263,9 +261,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -289,7 +287,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -324,7 +322,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -342,7 +340,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -367,7 +365,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -403,74 +401,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B5D223-5ABE-D343-A7F1-A29E0BE91818}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B5D223-5ABE-D343-A7F1-A29E0BE91818}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="true" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="true"/>
-    <col min="5" max="5" width="2.7109375" customWidth="true"/>
-    <col min="6" max="9" width="2.6640625" customWidth="true"/>
-    <col min="10" max="10" width="6.6640625" customWidth="true"/>
-    <col min="11" max="14" width="2.6640625" customWidth="true"/>
-    <col min="2" max="2" width="2.7109375" customWidth="true"/>
-    <col min="3" max="3" width="2.7109375" customWidth="true"/>
-    <col min="4" max="4" width="2.7109375" customWidth="true"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="5" width="2.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" customWidth="1"/>
+    <col min="7" max="9" width="2.6640625" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" customWidth="1"/>
+    <col min="11" max="14" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="0">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" s="0">
+      <c r="B1">
         <v>2</v>
       </c>
-      <c r="C1" s="0">
+      <c r="C1">
         <v>3</v>
       </c>
-      <c r="D1" s="0">
+      <c r="D1">
         <v>4</v>
       </c>
-      <c r="E1" s="0">
+      <c r="E1">
         <v>5</v>
       </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>35932</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="C2" s="0">
+      <c r="F2">
+        <v>0.85699999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>39634</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="E2" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>3048</v>
-      </c>
-      <c r="B3" s="0">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0">
-        <v>1</v>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>491.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>